<commit_message>
Getting many things sorted
</commit_message>
<xml_diff>
--- a/data/data_scats.xlsx
+++ b/data/data_scats.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C78B0C4-15DB-4DAB-856D-2DB817C9CFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8062EAB8-7501-4EA2-9326-8F3628B68D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="157">
   <si>
     <t>Code_sample</t>
   </si>
@@ -341,6 +341,165 @@
   </si>
   <si>
     <t>Cap Noir</t>
+  </si>
+  <si>
+    <t>marron clair</t>
+  </si>
+  <si>
+    <t>quasi que du poil!! Avec des petites dents (pas de poisson, mamm? Tout petit), des griffes pointues (toutes petites, blanches, pas otaries), pi_ces NA et plumes manchots</t>
+  </si>
+  <si>
+    <t>marron foncé</t>
+  </si>
+  <si>
+    <t>poils</t>
+  </si>
+  <si>
+    <t>noire</t>
+  </si>
+  <si>
+    <t>très peu de matière - cristaux + poils</t>
+  </si>
+  <si>
+    <t>gras ?</t>
+  </si>
+  <si>
+    <t>marron</t>
+  </si>
+  <si>
+    <t>os ? Plumes manchots - poils</t>
+  </si>
+  <si>
+    <t>grise</t>
+  </si>
+  <si>
+    <t>crustacés ? (uniquement)</t>
+  </si>
+  <si>
+    <t>gras+pup??</t>
+  </si>
+  <si>
+    <t>marron foncé/clair</t>
+  </si>
+  <si>
+    <t>poils-otolithes-cristallins céphalopodes</t>
+  </si>
+  <si>
+    <t>poils-cailloux</t>
+  </si>
+  <si>
+    <t>0-1? cristaux + résidus crustacés ?</t>
+  </si>
+  <si>
+    <t>cailloux + crustacés uniquement</t>
+  </si>
+  <si>
+    <t>poils-cailloux-otolithes-cristallins céphalopodes</t>
+  </si>
+  <si>
+    <t>0-1? cailloux, sec + résidus Leptplu / poils + résidus crustacés ?</t>
+  </si>
+  <si>
+    <t>otolithes+cristallins+poils</t>
+  </si>
+  <si>
+    <t>otolithes+cristallins</t>
+  </si>
+  <si>
+    <t>très très peu de matière - brillant, pup?</t>
+  </si>
+  <si>
+    <t>marron clair/gris</t>
+  </si>
+  <si>
+    <t>quasi que du poil, en boule autour de plumes de manchots!!</t>
+  </si>
+  <si>
+    <t>mélange marron foncé/clair/gris</t>
+  </si>
+  <si>
+    <t>poils+vertèbres</t>
+  </si>
+  <si>
+    <t>marron brun</t>
+  </si>
+  <si>
+    <t>0-1? résidus crustacés ?</t>
+  </si>
+  <si>
+    <t>poisson+céphalo+poils+cailloux</t>
+  </si>
+  <si>
+    <t>cailloux</t>
+  </si>
+  <si>
+    <t>otolithes+cristallins+cailloux(+++!)</t>
+  </si>
+  <si>
+    <t>poils+otolithes+cailloux</t>
+  </si>
+  <si>
+    <t>0-1? rien ou résidus crustacés?</t>
+  </si>
+  <si>
+    <t>mélange marron foncé/clair</t>
+  </si>
+  <si>
+    <t>otolithes+cristallins(+)+poils</t>
+  </si>
+  <si>
+    <t>marron foncé/noire</t>
+  </si>
+  <si>
+    <t>sec - résidus plantes</t>
+  </si>
+  <si>
+    <t>otolithes+cristallins(+)</t>
+  </si>
+  <si>
+    <t>otolithes+cristallins+arrêtes/vert</t>
+  </si>
+  <si>
+    <t>cristaux + résidus crustacés ?</t>
+  </si>
+  <si>
+    <t>cailloux+otolithes+cristallins</t>
+  </si>
+  <si>
+    <t>0-1? cailloux+poils+résidus crustacés ?</t>
+  </si>
+  <si>
+    <t>"brillant"+crustacés ?</t>
+  </si>
+  <si>
+    <t>marron clair-grise</t>
+  </si>
+  <si>
+    <t>poils+gras?</t>
+  </si>
+  <si>
+    <t>très peu de matière - gras aussi un peu… pup?</t>
+  </si>
+  <si>
+    <t>poils+cailloux</t>
+  </si>
+  <si>
+    <t>cristaux</t>
+  </si>
+  <si>
+    <t>résidus Leptplu</t>
+  </si>
+  <si>
+    <t>index_hard_parts</t>
+  </si>
+  <si>
+    <t>color_hard_parts</t>
+  </si>
+  <si>
+    <t>comments_hard_parts</t>
+  </si>
+  <si>
+    <t>pup_suspicion</t>
   </si>
 </sst>
 </file>
@@ -677,13 +836,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="K4" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.36328125" customWidth="1"/>
@@ -695,9 +854,12 @@
     <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="79.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -737,8 +899,20 @@
       <c r="M1" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -778,8 +952,17 @@
         <f>100*(J2-K2)/J2</f>
         <v>59.121721190686713</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -822,8 +1005,17 @@
       <c r="M3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -866,8 +1058,20 @@
       <c r="M4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4" t="s">
+        <v>106</v>
+      </c>
+      <c r="P4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -910,8 +1114,20 @@
       <c r="M5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>108</v>
+      </c>
+      <c r="P5" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -951,8 +1167,20 @@
         <f t="shared" si="2"/>
         <v>58.920800696257629</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>108</v>
+      </c>
+      <c r="P6" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -992,8 +1220,20 @@
       <c r="M7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>111</v>
+      </c>
+      <c r="P7" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1033,8 +1273,17 @@
         <f t="shared" si="2"/>
         <v>67.084793272599867</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1074,8 +1323,17 @@
         <f t="shared" si="2"/>
         <v>66.94734297570605</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1118,8 +1376,20 @@
       <c r="M10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10" t="s">
+        <v>108</v>
+      </c>
+      <c r="P10" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1162,8 +1432,20 @@
       <c r="M11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>111</v>
+      </c>
+      <c r="P11" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1206,8 +1488,20 @@
       <c r="M12" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12" t="s">
+        <v>116</v>
+      </c>
+      <c r="P12" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1247,8 +1541,17 @@
         <f t="shared" si="2"/>
         <v>64.326341983647353</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1291,8 +1594,20 @@
       <c r="M14" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>108</v>
+      </c>
+      <c r="P14" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1332,8 +1647,20 @@
       <c r="M15" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15" t="s">
+        <v>108</v>
+      </c>
+      <c r="P15" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1370,8 +1697,20 @@
         <f t="shared" si="2"/>
         <v>57.571109871723372</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16" t="s">
+        <v>108</v>
+      </c>
+      <c r="P16" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1411,8 +1750,17 @@
         <f t="shared" si="2"/>
         <v>41.209640745793564</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1449,8 +1797,17 @@
         <f t="shared" si="2"/>
         <v>66.885325558794946</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1487,8 +1844,20 @@
         <f t="shared" si="2"/>
         <v>54.470836057238323</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19" t="s">
+        <v>108</v>
+      </c>
+      <c r="P19" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1528,8 +1897,17 @@
         <f t="shared" si="2"/>
         <v>40.087108013937282</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N20">
+        <v>3</v>
+      </c>
+      <c r="O20" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1569,8 +1947,17 @@
         <f t="shared" si="2"/>
         <v>54.478534200204173</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N21">
+        <v>3</v>
+      </c>
+      <c r="O21" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1607,8 +1994,17 @@
         <f t="shared" si="2"/>
         <v>61.603960396039589</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N22">
+        <v>3</v>
+      </c>
+      <c r="O22" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1648,8 +2044,20 @@
         <f t="shared" si="2"/>
         <v>61.170701808151961</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>111</v>
+      </c>
+      <c r="P23" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1689,8 +2097,20 @@
         <f t="shared" si="2"/>
         <v>33.816595115771698</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24" t="s">
+        <v>108</v>
+      </c>
+      <c r="P24" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1730,8 +2150,20 @@
         <f t="shared" si="2"/>
         <v>55.477242269320492</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25" t="s">
+        <v>104</v>
+      </c>
+      <c r="P25" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1768,8 +2200,20 @@
         <f t="shared" si="2"/>
         <v>55.997477235996683</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N26">
+        <v>2</v>
+      </c>
+      <c r="O26" t="s">
+        <v>113</v>
+      </c>
+      <c r="P26" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1809,8 +2253,20 @@
         <f t="shared" si="2"/>
         <v>52.905811623246301</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27" t="s">
+        <v>104</v>
+      </c>
+      <c r="P27" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1850,8 +2306,20 @@
       <c r="M28" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28" t="s">
+        <v>126</v>
+      </c>
+      <c r="P28" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1888,8 +2356,17 @@
         <f t="shared" si="2"/>
         <v>55.713619402985103</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N29">
+        <v>2</v>
+      </c>
+      <c r="O29" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1929,8 +2406,17 @@
         <f t="shared" si="2"/>
         <v>50.443599493029154</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N30">
+        <v>2</v>
+      </c>
+      <c r="O30" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1967,8 +2453,20 @@
         <f t="shared" si="2"/>
         <v>33.619631901840457</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31" t="s">
+        <v>106</v>
+      </c>
+      <c r="P31" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2005,8 +2503,17 @@
         <f t="shared" si="2"/>
         <v>44.426516068307137</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N32">
+        <v>2</v>
+      </c>
+      <c r="O32" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2046,8 +2553,17 @@
         <f t="shared" si="2"/>
         <v>55.911792905081498</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N33">
+        <v>2</v>
+      </c>
+      <c r="O33" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2090,8 +2606,20 @@
       <c r="M34" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34" t="s">
+        <v>108</v>
+      </c>
+      <c r="P34" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2131,8 +2659,20 @@
         <f t="shared" si="2"/>
         <v>54.321618308132422</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N35">
+        <v>2</v>
+      </c>
+      <c r="O35" t="s">
+        <v>111</v>
+      </c>
+      <c r="P35" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2175,8 +2715,17 @@
       <c r="M36" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N36">
+        <v>2</v>
+      </c>
+      <c r="O36" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2219,8 +2768,20 @@
       <c r="M37" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37" t="s">
+        <v>106</v>
+      </c>
+      <c r="P37" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2260,8 +2821,17 @@
         <f t="shared" si="2"/>
         <v>50.746575342465754</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N38">
+        <v>2</v>
+      </c>
+      <c r="O38" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2304,8 +2874,20 @@
       <c r="M39" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N39">
+        <v>3</v>
+      </c>
+      <c r="O39" t="s">
+        <v>106</v>
+      </c>
+      <c r="P39" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2345,8 +2927,20 @@
         <f t="shared" si="2"/>
         <v>37.38833847653077</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N40">
+        <v>2</v>
+      </c>
+      <c r="O40" t="s">
+        <v>106</v>
+      </c>
+      <c r="P40" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2386,8 +2980,20 @@
         <f t="shared" si="2"/>
         <v>35.807942646920125</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41" t="s">
+        <v>108</v>
+      </c>
+      <c r="P41" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2427,8 +3033,20 @@
         <f t="shared" si="2"/>
         <v>61.824953445065219</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42" t="s">
+        <v>104</v>
+      </c>
+      <c r="P42" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2468,8 +3086,20 @@
         <f t="shared" si="2"/>
         <v>51.618286940454205</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N43">
+        <v>2</v>
+      </c>
+      <c r="O43" t="s">
+        <v>137</v>
+      </c>
+      <c r="P43" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2509,8 +3139,20 @@
         <f t="shared" si="2"/>
         <v>47.153330213695206</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44" t="s">
+        <v>139</v>
+      </c>
+      <c r="P44" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2550,8 +3192,20 @@
         <f t="shared" si="2"/>
         <v>57.780535821278775</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N45">
+        <v>3</v>
+      </c>
+      <c r="O45" t="s">
+        <v>137</v>
+      </c>
+      <c r="P45" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2594,8 +3248,20 @@
       <c r="M46" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N46">
+        <v>3</v>
+      </c>
+      <c r="O46" t="s">
+        <v>113</v>
+      </c>
+      <c r="P46" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2638,8 +3304,20 @@
       <c r="M47" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47" t="s">
+        <v>108</v>
+      </c>
+      <c r="P47" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2679,8 +3357,20 @@
         <f t="shared" si="2"/>
         <v>43.537906137184102</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48" t="s">
+        <v>106</v>
+      </c>
+      <c r="P48" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2720,8 +3410,20 @@
         <f t="shared" si="2"/>
         <v>17.094850948509471</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N49">
+        <v>3</v>
+      </c>
+      <c r="O49" t="s">
+        <v>104</v>
+      </c>
+      <c r="P49" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2764,8 +3466,17 @@
       <c r="M50" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N50">
+        <v>3</v>
+      </c>
+      <c r="O50" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2808,8 +3519,20 @@
       <c r="M51" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51" t="s">
+        <v>108</v>
+      </c>
+      <c r="P51" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2846,8 +3569,17 @@
         <f t="shared" si="2"/>
         <v>54.588918677390531</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N52">
+        <v>3</v>
+      </c>
+      <c r="O52" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2887,8 +3619,20 @@
         <f t="shared" si="2"/>
         <v>60.029211295034081</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N53">
+        <v>2</v>
+      </c>
+      <c r="O53" t="s">
+        <v>111</v>
+      </c>
+      <c r="P53" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2928,8 +3672,17 @@
         <f t="shared" si="2"/>
         <v>23.293951684006348</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N54">
+        <v>3</v>
+      </c>
+      <c r="O54" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2966,8 +3719,20 @@
         <f t="shared" si="2"/>
         <v>60.986285380799544</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55" t="s">
+        <v>106</v>
+      </c>
+      <c r="P55" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -3007,8 +3772,20 @@
         <f t="shared" si="2"/>
         <v>43.012211668927861</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56" t="s">
+        <v>111</v>
+      </c>
+      <c r="P56" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -3045,8 +3822,20 @@
         <f t="shared" si="2"/>
         <v>29.014900662251648</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N57">
+        <v>2</v>
+      </c>
+      <c r="O57" t="s">
+        <v>106</v>
+      </c>
+      <c r="P57" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -3083,8 +3872,20 @@
         <f t="shared" si="2"/>
         <v>18.117854001759042</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58" t="s">
+        <v>108</v>
+      </c>
+      <c r="P58" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -3121,8 +3922,17 @@
         <f t="shared" si="2"/>
         <v>31.703861140630515</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N59">
+        <v>2</v>
+      </c>
+      <c r="O59" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -3159,8 +3969,20 @@
         <f t="shared" si="2"/>
         <v>30.96085409252672</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60" t="s">
+        <v>108</v>
+      </c>
+      <c r="P60" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -3196,6 +4018,15 @@
       <c r="L61">
         <f t="shared" si="2"/>
         <v>38.832092454717191</v>
+      </c>
+      <c r="N61">
+        <v>3</v>
+      </c>
+      <c r="O61" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q61">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>